<commit_message>
ths is the robot code
</commit_message>
<xml_diff>
--- a/Curt/distance data points vision tracking.xlsx
+++ b/Curt/distance data points vision tracking.xlsx
@@ -142,8 +142,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="7.0094352712887636E-2"/>
-          <c:y val="0.12217614213733763"/>
-          <c:w val="0.88082285697186058"/>
+          <c:y val="0.12217614213733764"/>
+          <c:w val="0.88082285697186069"/>
           <c:h val="0.80150161157686972"/>
         </c:manualLayout>
       </c:layout>
@@ -163,8 +163,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="5.8083623389270003E-3"/>
-                  <c:y val="3.0269482136397265E-2"/>
+                  <c:x val="5.8083623389270011E-3"/>
+                  <c:y val="3.0269482136397262E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -237,23 +237,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="71532544"/>
-        <c:axId val="69756800"/>
+        <c:axId val="91424640"/>
+        <c:axId val="91426176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71532544"/>
+        <c:axId val="91424640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69756800"/>
+        <c:crossAx val="91426176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69756800"/>
+        <c:axId val="91426176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -261,7 +261,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71532544"/>
+        <c:crossAx val="91424640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -272,9 +272,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.2407176014450578E-2"/>
-          <c:y val="9.2455766796814484E-3"/>
-          <c:w val="0.20954225103118959"/>
+          <c:x val="8.2407176014450564E-2"/>
+          <c:y val="9.2455766796814519E-3"/>
+          <c:w val="0.20954225103118962"/>
           <c:h val="0.11018263258446265"/>
         </c:manualLayout>
       </c:layout>
@@ -283,7 +283,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -299,10 +299,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="6.8722629133036936E-2"/>
-          <c:y val="0.12653889018040482"/>
-          <c:w val="0.88093724170292831"/>
-          <c:h val="0.80158293915739998"/>
+          <c:x val="6.8722629133036964E-2"/>
+          <c:y val="0.12653889018040487"/>
+          <c:w val="0.88093724170292809"/>
+          <c:h val="0.80158293915739987"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -322,7 +322,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="5.6629108937207477E-3"/>
-                  <c:y val="-5.164263882233628E-2"/>
+                  <c:y val="-5.1642638822336301E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -395,23 +395,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="73047040"/>
-        <c:axId val="73044736"/>
+        <c:axId val="91450752"/>
+        <c:axId val="91468928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73047040"/>
+        <c:axId val="91450752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73044736"/>
+        <c:crossAx val="91468928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73044736"/>
+        <c:axId val="91468928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -419,7 +419,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73047040"/>
+        <c:crossAx val="91450752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -430,10 +430,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.4839056639063118E-2"/>
-          <c:y val="1.7736617955806628E-2"/>
-          <c:w val="0.20544157764467824"/>
-          <c:h val="0.1037669415449347"/>
+          <c:x val="8.4839056639063146E-2"/>
+          <c:y val="1.7736617955806624E-2"/>
+          <c:w val="0.20544157764467821"/>
+          <c:h val="0.10376694154493472"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -441,7 +441,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -457,9 +457,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="6.4082615636373172E-2"/>
-          <c:y val="0.11929079204458277"/>
-          <c:w val="0.89518049942165734"/>
+          <c:x val="6.4082615636373186E-2"/>
+          <c:y val="0.11929079204458279"/>
+          <c:w val="0.89518049942165723"/>
           <c:h val="0.81294819079472813"/>
         </c:manualLayout>
       </c:layout>
@@ -479,7 +479,7 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-4.2870475178978457E-3"/>
+                  <c:x val="-4.2870475178978466E-3"/>
                   <c:y val="4.2614625028699123E-2"/>
                 </c:manualLayout>
               </c:layout>
@@ -553,23 +553,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="72456832"/>
-        <c:axId val="72455296"/>
+        <c:axId val="95302784"/>
+        <c:axId val="95304320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72456832"/>
+        <c:axId val="95302784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72455296"/>
+        <c:crossAx val="95304320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72455296"/>
+        <c:axId val="95304320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -577,7 +577,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72456832"/>
+        <c:crossAx val="95302784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -588,9 +588,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.10733447291999787"/>
+          <c:x val="0.10733447291999788"/>
           <c:y val="2.0829490810531474E-3"/>
-          <c:w val="0.19157057612635961"/>
+          <c:w val="0.19157057612635958"/>
           <c:h val="9.7823211720060158E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -599,7 +599,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -629,8 +629,21 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="6.2448760115567846E-2"/>
-                  <c:y val="-0.15050167455442831"/>
+                  <c:x val="6.2448760115567853E-2"/>
+                  <c:y val="-0.15050167455442834"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.11232134001641082"/>
+                  <c:y val="-6.4204012474069996E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -703,23 +716,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="74062848"/>
-        <c:axId val="74061312"/>
+        <c:axId val="95324800"/>
+        <c:axId val="95334784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="74062848"/>
+        <c:axId val="95324800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74061312"/>
+        <c:crossAx val="95334784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="74061312"/>
+        <c:axId val="95334784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -727,7 +740,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74062848"/>
+        <c:crossAx val="95324800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -739,8 +752,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.73589758048493581"/>
-          <c:y val="0.11459560271507487"/>
-          <c:w val="0.21227694895132915"/>
+          <c:y val="0.11459560271507489"/>
+          <c:w val="0.2122769489513292"/>
           <c:h val="0.10591199342537926"/>
         </c:manualLayout>
       </c:layout>
@@ -749,7 +762,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -855,9 +868,9 @@
       <xdr:rowOff>22412</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>515469</xdr:colOff>
-      <xdr:row>134</xdr:row>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>481853</xdr:colOff>
+      <xdr:row>137</xdr:row>
       <xdr:rowOff>168088</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1167,7 +1180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:U126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="Q136" sqref="Q136"/>
     </sheetView>
   </sheetViews>
@@ -1326,7 +1339,7 @@
         <v>223.8</v>
       </c>
       <c r="L8">
-        <f>E8-G8</f>
+        <f t="shared" ref="L8:L13" si="0">E8-G8</f>
         <v>63.099999999999994</v>
       </c>
       <c r="O8" s="3"/>
@@ -1356,7 +1369,7 @@
         <v>227.2</v>
       </c>
       <c r="L9">
-        <f>E9-G9</f>
+        <f t="shared" si="0"/>
         <v>48.700000000000017</v>
       </c>
       <c r="O9" s="3"/>
@@ -1386,7 +1399,7 @@
         <v>215.3</v>
       </c>
       <c r="L10">
-        <f>E10-G10</f>
+        <f t="shared" si="0"/>
         <v>38.5</v>
       </c>
       <c r="O10" s="3"/>
@@ -1416,7 +1429,7 @@
         <v>213.2</v>
       </c>
       <c r="L11">
-        <f>E11-G11</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="O11" s="4"/>
@@ -1448,7 +1461,7 @@
         <v>208.3</v>
       </c>
       <c r="L12">
-        <f>E12-G12</f>
+        <f t="shared" si="0"/>
         <v>27.700000000000017</v>
       </c>
       <c r="N12" t="s">
@@ -1482,7 +1495,7 @@
         <v>203.1</v>
       </c>
       <c r="L13">
-        <f>E13-G13</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Curt: Git hub is forcing me to do this
binaries differ so inorder to sync i must do this
</commit_message>
<xml_diff>
--- a/Curt/distance data points vision tracking.xlsx
+++ b/Curt/distance data points vision tracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="20115" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>Rectangle track at set distances</t>
   </si>
@@ -73,6 +73,30 @@
   </si>
   <si>
     <t>the height graph of left side</t>
+  </si>
+  <si>
+    <t>inches</t>
+  </si>
+  <si>
+    <t>5 ft</t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t>10 ft</t>
+  </si>
+  <si>
+    <t>this is new way to find distance</t>
+  </si>
+  <si>
+    <t>y1</t>
+  </si>
+  <si>
+    <t>y2</t>
+  </si>
+  <si>
+    <t>pixels</t>
   </si>
 </sst>
 </file>
@@ -142,7 +166,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="7.0094352712887636E-2"/>
-          <c:y val="0.12217614213733764"/>
+          <c:y val="0.12217614213733767"/>
           <c:w val="0.88082285697186069"/>
           <c:h val="0.80150161157686972"/>
         </c:manualLayout>
@@ -163,8 +187,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="5.8083623389270011E-3"/>
-                  <c:y val="3.0269482136397262E-2"/>
+                  <c:x val="5.8083623389270029E-3"/>
+                  <c:y val="3.0269482136397255E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -237,23 +261,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="91424640"/>
-        <c:axId val="91426176"/>
+        <c:axId val="97344896"/>
+        <c:axId val="97354880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91424640"/>
+        <c:axId val="97344896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91426176"/>
+        <c:crossAx val="97354880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91426176"/>
+        <c:axId val="97354880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -261,7 +285,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91424640"/>
+        <c:crossAx val="97344896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -272,9 +296,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.2407176014450564E-2"/>
-          <c:y val="9.2455766796814519E-3"/>
-          <c:w val="0.20954225103118962"/>
+          <c:x val="8.2407176014450551E-2"/>
+          <c:y val="9.2455766796814571E-3"/>
+          <c:w val="0.20954225103118973"/>
           <c:h val="0.11018263258446265"/>
         </c:manualLayout>
       </c:layout>
@@ -283,7 +307,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -299,10 +323,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="6.8722629133036964E-2"/>
-          <c:y val="0.12653889018040487"/>
-          <c:w val="0.88093724170292809"/>
-          <c:h val="0.80158293915739987"/>
+          <c:x val="6.8722629133037005E-2"/>
+          <c:y val="0.12653889018040496"/>
+          <c:w val="0.88093724170292764"/>
+          <c:h val="0.80158293915739953"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -322,7 +346,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="5.6629108937207477E-3"/>
-                  <c:y val="-5.1642638822336301E-2"/>
+                  <c:y val="-5.1642638822336336E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -395,23 +419,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="91450752"/>
-        <c:axId val="91468928"/>
+        <c:axId val="97383552"/>
+        <c:axId val="97385088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91450752"/>
+        <c:axId val="97383552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91468928"/>
+        <c:crossAx val="97385088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91468928"/>
+        <c:axId val="97385088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -419,7 +443,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91450752"/>
+        <c:crossAx val="97383552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -430,10 +454,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.4839056639063146E-2"/>
-          <c:y val="1.7736617955806624E-2"/>
-          <c:w val="0.20544157764467821"/>
-          <c:h val="0.10376694154493472"/>
+          <c:x val="8.4839056639063173E-2"/>
+          <c:y val="1.7736617955806618E-2"/>
+          <c:w val="0.20544157764467819"/>
+          <c:h val="0.10376694154493477"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -441,7 +465,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -457,9 +481,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="6.4082615636373186E-2"/>
-          <c:y val="0.11929079204458279"/>
-          <c:w val="0.89518049942165723"/>
+          <c:x val="6.4082615636373214E-2"/>
+          <c:y val="0.11929079204458283"/>
+          <c:w val="0.89518049942165701"/>
           <c:h val="0.81294819079472813"/>
         </c:manualLayout>
       </c:layout>
@@ -479,7 +503,7 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-4.2870475178978466E-3"/>
+                  <c:x val="-4.2870475178978474E-3"/>
                   <c:y val="4.2614625028699123E-2"/>
                 </c:manualLayout>
               </c:layout>
@@ -553,23 +577,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="95302784"/>
-        <c:axId val="95304320"/>
+        <c:axId val="118774400"/>
+        <c:axId val="118784384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95302784"/>
+        <c:axId val="118774400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95304320"/>
+        <c:crossAx val="118784384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95304320"/>
+        <c:axId val="118784384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -577,7 +601,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95302784"/>
+        <c:crossAx val="118774400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -588,9 +612,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.10733447291999788"/>
+          <c:x val="0.10733447291999791"/>
           <c:y val="2.0829490810531474E-3"/>
-          <c:w val="0.19157057612635958"/>
+          <c:w val="0.19157057612635953"/>
           <c:h val="9.7823211720060158E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -599,7 +623,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -610,7 +634,17 @@
   <c:lang val="en-US"/>
   <c:chart>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.8766735077795854E-2"/>
+          <c:y val="4.1665580044399388E-2"/>
+          <c:w val="0.69952816754809333"/>
+          <c:h val="0.94254403265082609"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:ser>
@@ -630,7 +664,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="6.2448760115567853E-2"/>
-                  <c:y val="-0.15050167455442834"/>
+                  <c:y val="-0.15050167455442842"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -642,8 +676,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.11232134001641082"/>
-                  <c:y val="-6.4204012474069996E-2"/>
+                  <c:x val="-0.11232134001641086"/>
+                  <c:y val="-6.4204012474069969E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -716,23 +750,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="95324800"/>
-        <c:axId val="95334784"/>
+        <c:axId val="118801536"/>
+        <c:axId val="118803072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95324800"/>
+        <c:axId val="118801536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95334784"/>
+        <c:crossAx val="118803072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95334784"/>
+        <c:axId val="118803072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -740,7 +774,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95324800"/>
+        <c:crossAx val="118801536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -752,11 +786,535 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.73589758048493581"/>
-          <c:y val="0.11459560271507489"/>
-          <c:w val="0.2122769489513292"/>
+          <c:y val="0.11459560271507493"/>
+          <c:w val="0.21227694895132926"/>
           <c:h val="0.10591199342537926"/>
         </c:manualLayout>
       </c:layout>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="exp"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.6677165354330718E-2"/>
+                  <c:y val="3.3206687013124674E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.0156167979002622E-2"/>
+                  <c:y val="-0.33024020548975563"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$115:$P$122</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>186.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>63.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$Q$115:$Q$122</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="118816128"/>
+        <c:axId val="119313536"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="118816128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="119313536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="119313536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="118816128"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="exp"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$139:$A$144</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$139:$B$144</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4.1340653334175297</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.088878535656402</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70.653227792630403</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>292.08505971156529</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1207.4987197627713</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4991.8785975173214</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="119333248"/>
+        <c:axId val="119334784"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="119333248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="119334784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="119334784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="119333248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$T$134</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>distance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$S$135:$S$138</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$T$135:$T$138</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5.9778599999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.9390000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.07</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="119371648"/>
+        <c:axId val="119373184"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="119371648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="119373184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="119373184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="119371648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$T$149</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>distance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+          </c:trendline>
+          <c:trendline>
+            <c:trendlineType val="exp"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.14527996500437446"/>
+                  <c:y val="8.7814671668413197E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$S$150:$S$153</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$T$150:$T$153</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>9.7640999999999991</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.7799999999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.7919999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.9779999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="119419648"/>
+        <c:axId val="119421184"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="119419648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="119421184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="119421184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="119419648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -863,15 +1421,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>268941</xdr:colOff>
-      <xdr:row>112</xdr:row>
-      <xdr:rowOff>22412</xdr:rowOff>
+      <xdr:colOff>246529</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>481853</xdr:colOff>
-      <xdr:row>137</xdr:row>
-      <xdr:rowOff>168088</xdr:rowOff>
+      <xdr:colOff>459441</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -885,6 +1443,126 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>67235</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>403411</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>336176</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>67235</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>145676</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>291353</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>168088</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>22412</xdr:colOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>56029</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>134471</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>33617</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>470647</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>112058</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1178,10 +1856,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:U126"/>
+  <dimension ref="A2:U153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q136" sqref="Q136"/>
+    <sheetView topLeftCell="A112" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1761,73 +2439,121 @@
         <v>203.1</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
+    <row r="114" spans="1:17">
       <c r="A114" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
+    <row r="115" spans="1:17">
       <c r="A115" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:2">
+      <c r="P115">
+        <v>186.9</v>
+      </c>
+      <c r="Q115" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:17">
       <c r="A116" s="1">
         <v>5</v>
       </c>
       <c r="B116">
         <v>186.9</v>
       </c>
-    </row>
-    <row r="117" spans="1:2">
+      <c r="P116">
+        <v>97.6</v>
+      </c>
+      <c r="Q116" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="117" spans="1:17">
       <c r="A117" s="1">
         <v>10</v>
       </c>
       <c r="B117">
         <v>97.6</v>
       </c>
-    </row>
-    <row r="118" spans="1:2">
+      <c r="P117">
+        <v>63.1</v>
+      </c>
+      <c r="Q117" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="118" spans="1:17">
       <c r="A118" s="1">
         <v>15</v>
       </c>
       <c r="B118">
         <v>63.1</v>
       </c>
-    </row>
-    <row r="119" spans="1:2">
+      <c r="P118">
+        <v>48.7</v>
+      </c>
+      <c r="Q118" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="119" spans="1:17">
       <c r="A119" s="1">
         <v>20</v>
       </c>
       <c r="B119">
         <v>48.7</v>
       </c>
-    </row>
-    <row r="120" spans="1:2">
+      <c r="P119">
+        <v>38.5</v>
+      </c>
+      <c r="Q119" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="120" spans="1:17">
       <c r="A120" s="1">
         <v>25</v>
       </c>
       <c r="B120">
         <v>38.5</v>
       </c>
-    </row>
-    <row r="121" spans="1:2">
+      <c r="P120">
+        <v>32</v>
+      </c>
+      <c r="Q120" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="121" spans="1:17">
       <c r="A121" s="1">
         <v>30</v>
       </c>
       <c r="B121">
         <v>32</v>
       </c>
-    </row>
-    <row r="122" spans="1:2">
+      <c r="P121">
+        <v>27.7</v>
+      </c>
+      <c r="Q121" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="122" spans="1:17">
       <c r="A122" s="1">
         <v>35</v>
       </c>
       <c r="B122">
         <v>27.7</v>
       </c>
-    </row>
-    <row r="123" spans="1:2">
+      <c r="P122">
+        <v>24</v>
+      </c>
+      <c r="Q122" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="123" spans="1:17">
       <c r="A123" s="1">
         <v>40</v>
       </c>
@@ -1835,14 +2561,168 @@
         <v>24</v>
       </c>
     </row>
-    <row r="124" spans="1:2">
+    <row r="124" spans="1:17">
       <c r="A124" s="1"/>
     </row>
-    <row r="125" spans="1:2">
+    <row r="125" spans="1:17">
       <c r="A125" s="1"/>
     </row>
-    <row r="126" spans="1:2">
+    <row r="126" spans="1:17">
       <c r="A126" s="1"/>
+    </row>
+    <row r="133" spans="1:20">
+      <c r="S133" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="134" spans="1:20">
+      <c r="S134" t="s">
+        <v>19</v>
+      </c>
+      <c r="T134" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="135" spans="1:20">
+      <c r="S135">
+        <v>0</v>
+      </c>
+      <c r="T135">
+        <v>5.9778599999999997</v>
+      </c>
+    </row>
+    <row r="136" spans="1:20">
+      <c r="S136">
+        <v>6</v>
+      </c>
+      <c r="T136">
+        <v>6.01</v>
+      </c>
+    </row>
+    <row r="137" spans="1:20">
+      <c r="S137">
+        <v>12</v>
+      </c>
+      <c r="T137">
+        <v>5.9390000000000001</v>
+      </c>
+    </row>
+    <row r="138" spans="1:20">
+      <c r="S138">
+        <v>18</v>
+      </c>
+      <c r="T138">
+        <v>6.07</v>
+      </c>
+    </row>
+    <row r="139" spans="1:20">
+      <c r="A139" s="1">
+        <v>5</v>
+      </c>
+      <c r="B139">
+        <f xml:space="preserve"> 174.33^(A139*0.055)</f>
+        <v>4.1340653334175297</v>
+      </c>
+    </row>
+    <row r="140" spans="1:20">
+      <c r="A140" s="1">
+        <v>10</v>
+      </c>
+      <c r="B140">
+        <f>174.3^(0.055*A140)</f>
+        <v>17.088878535656402</v>
+      </c>
+    </row>
+    <row r="141" spans="1:20">
+      <c r="A141" s="1">
+        <v>15</v>
+      </c>
+      <c r="B141">
+        <f>174.33^(0.055*A141)</f>
+        <v>70.653227792630403</v>
+      </c>
+    </row>
+    <row r="142" spans="1:20">
+      <c r="A142" s="1">
+        <v>20</v>
+      </c>
+      <c r="B142">
+        <f>174.33^(0.055*A142)</f>
+        <v>292.08505971156529</v>
+      </c>
+    </row>
+    <row r="143" spans="1:20">
+      <c r="A143" s="1">
+        <v>25</v>
+      </c>
+      <c r="B143">
+        <f>174.33^(0.055*A143)</f>
+        <v>1207.4987197627713</v>
+      </c>
+    </row>
+    <row r="144" spans="1:20">
+      <c r="A144" s="1">
+        <v>30</v>
+      </c>
+      <c r="B144">
+        <f>174.33^(0.055*A144)</f>
+        <v>4991.8785975173214</v>
+      </c>
+    </row>
+    <row r="145" spans="1:20">
+      <c r="A145" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="146" spans="1:20">
+      <c r="A146" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="148" spans="1:20">
+      <c r="S148" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="149" spans="1:20">
+      <c r="S149" t="s">
+        <v>19</v>
+      </c>
+      <c r="T149" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="150" spans="1:20">
+      <c r="S150">
+        <v>0</v>
+      </c>
+      <c r="T150">
+        <v>9.7640999999999991</v>
+      </c>
+    </row>
+    <row r="151" spans="1:20">
+      <c r="S151">
+        <v>6</v>
+      </c>
+      <c r="T151">
+        <v>9.7799999999999994</v>
+      </c>
+    </row>
+    <row r="152" spans="1:20">
+      <c r="S152">
+        <v>12</v>
+      </c>
+      <c r="T152">
+        <v>9.7919999999999998</v>
+      </c>
+    </row>
+    <row r="153" spans="1:20">
+      <c r="S153">
+        <v>18</v>
+      </c>
+      <c r="T153">
+        <v>9.9779999999999998</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1853,12 +2733,104 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>431</v>
+      </c>
+      <c r="C4">
+        <v>361</v>
+      </c>
+      <c r="D4">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>407</v>
+      </c>
+      <c r="C5">
+        <v>338</v>
+      </c>
+      <c r="D5">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>374</v>
+      </c>
+      <c r="C6">
+        <v>308.39999999999998</v>
+      </c>
+      <c r="D6">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>345</v>
+      </c>
+      <c r="C7">
+        <v>282.8</v>
+      </c>
+      <c r="D7">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>310.5</v>
+      </c>
+      <c r="C8">
+        <v>250</v>
+      </c>
+      <c r="D8">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>